<commit_message>
calculator fixtures: split merged cells
</commit_message>
<xml_diff>
--- a/public/local/fixtures/calculator/Мониторинг калькуляторы.xlsx
+++ b/public/local/fixtures/calculator/Мониторинг калькуляторы.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37520" windowHeight="21140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37520" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Мониторинг одного здания" sheetId="3" r:id="rId1"/>
     <sheet name="Мониторинг нескольких зданий" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1207,7 +1207,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1251,6 +1251,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1348,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1379,12 +1381,14 @@
     <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1663,7 +1667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1673,7 +1677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF249"/>
   <sheetViews>
-    <sheetView topLeftCell="A208" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
       <selection activeCell="A236" sqref="A236"/>
     </sheetView>
   </sheetViews>
@@ -5036,8 +5040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="A350" sqref="A350"/>
+    <sheetView topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="D261" sqref="D261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7788,7 +7792,9 @@
       <c r="B259" s="34">
         <v>1</v>
       </c>
-      <c r="C259" s="24"/>
+      <c r="C259" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260">
@@ -7797,7 +7803,9 @@
       <c r="B260" s="34">
         <v>2</v>
       </c>
-      <c r="C260" s="24"/>
+      <c r="C260" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261">
@@ -7817,7 +7825,9 @@
       <c r="B262" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C262" s="24"/>
+      <c r="C262" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="263" spans="1:3" ht="15" thickBot="1">
       <c r="B263" s="5"/>
@@ -8931,6 +8941,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>